<commit_message>
Fix workbook corruption: add empty rows to header-only tables and regenerate
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -2,38 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
-    <sheet name="Home" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Work_Queue" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Account_Detail" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Overrides" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Reconciliations" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Admin" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="tblAccounts_Current" sheetId="7" state="hidden" r:id="rId7"/>
-    <sheet name="tblStaff" sheetId="8" state="hidden" r:id="rId8"/>
-    <sheet name="tblRanges_Default" sheetId="9" state="hidden" r:id="rId9"/>
-    <sheet name="tblRangeOverrides" sheetId="10" state="hidden" r:id="rId10"/>
-    <sheet name="tblDigitMap" sheetId="11" state="hidden" r:id="rId11"/>
-    <sheet name="tblAllocations" sheetId="12" state="hidden" r:id="rId12"/>
-    <sheet name="tblNotes" sheetId="13" state="hidden" r:id="rId13"/>
-    <sheet name="tblNoteTypes" sheetId="14" state="hidden" r:id="rId14"/>
-    <sheet name="tblConfig" sheetId="15" state="hidden" r:id="rId15"/>
-    <sheet name="tblReconIssues" sheetId="16" state="hidden" r:id="rId16"/>
-    <sheet name="tblNoteSyncQueue" sheetId="17" state="hidden" r:id="rId17"/>
-    <sheet name="tblNoteSyncLog" sheetId="18" state="hidden" r:id="rId18"/>
-    <sheet name="Sheet2" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Sheet3" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="Sheet4" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Sheet5" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="Sheet6" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="Sheet7" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="Sheet8" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="Sheet9" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="Sheet10" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="Sheet11" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="Sheet12" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -161,8 +149,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="tblNoteSyncLog" displayName="tblNoteSyncLog" ref="A1:E1" headerRowCount="1">
-  <autoFilter ref="A1:E1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="tblNoteSyncLog" displayName="tblNoteSyncLog" ref="A1:E2" headerRowCount="1">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Log_ID"/>
     <tableColumn id="2" name="Note_ID"/>
@@ -175,8 +163,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="tblRangeOverrides" displayName="tblRangeOverrides" ref="A1:E1" headerRowCount="1">
-  <autoFilter ref="A1:E1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="tblRangeOverrides" displayName="tblRangeOverrides" ref="A1:E2" headerRowCount="1">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Override_ID"/>
     <tableColumn id="2" name="Account_Number"/>
@@ -296,8 +284,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="tblNoteSyncQueue" displayName="tblNoteSyncQueue" ref="A1:E1" headerRowCount="1">
-  <autoFilter ref="A1:E1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="tblNoteSyncQueue" displayName="tblNoteSyncQueue" ref="A1:E2" headerRowCount="1">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Queue_ID"/>
     <tableColumn id="2" name="Note_ID"/>
@@ -630,15 +618,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4551407</v>
+        <v>4793634</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Account_4551407</t>
+          <t>Account_4793634</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>86340.85000000001</v>
+        <v>68692.63</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -648,33 +636,33 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5100429</v>
+        <v>7023462</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Account_5100429</t>
+          <t>Account_7023462</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>97236.49000000001</v>
+        <v>26564.18</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Operations</t>
+          <t>Finance</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5729196</v>
+        <v>9908228</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Account_5729196</t>
+          <t>Account_9908228</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>81280</v>
+        <v>66334.47</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -684,33 +672,33 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5649234</v>
+        <v>7875135</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Account_5649234</t>
+          <t>Account_7875135</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5455.11</v>
+        <v>35264.25</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>Finance</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1883294</v>
+        <v>6221893</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Account_1883294</t>
+          <t>Account_6221893</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>89501.05</v>
+        <v>35567.02</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -720,51 +708,51 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2981593</v>
+        <v>8066951</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Account_2981593</t>
+          <t>Account_8066951</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>38802.13</v>
+        <v>28553.16</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>Accounting</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5293997</v>
+        <v>8359387</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Account_5293997</t>
+          <t>Account_8359387</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>28690.37</v>
+        <v>41694.15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>Operations</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8382057</v>
+        <v>7334640</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Account_8382057</t>
+          <t>Account_7334640</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9966.16</v>
+        <v>61750.77</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -774,33 +762,33 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5481551</v>
+        <v>2617691</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Account_5481551</t>
+          <t>Account_2617691</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>52717.36</v>
+        <v>18081.74</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>Operations</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8571538</v>
+        <v>4671827</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Account_8571538</t>
+          <t>Account_4671827</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>66051.33</v>
+        <v>38213.07</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -810,15 +798,15 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4982845</v>
+        <v>2511172</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Account_4982845</t>
+          <t>Account_2511172</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17976.65</v>
+        <v>78947.69</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -828,141 +816,141 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2094202</v>
+        <v>7150843</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Account_2094202</t>
+          <t>Account_7150843</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>32520.94</v>
+        <v>54212.04</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Operations</t>
+          <t>Accounting</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>9775371</v>
+        <v>4558819</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Account_9775371</t>
+          <t>Account_4558819</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>91236.17999999999</v>
+        <v>47383.55</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>Admin</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3038731</v>
+        <v>8796304</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Account_3038731</t>
+          <t>Account_8796304</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>75321.47</v>
+        <v>4984.18</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>Admin</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>8321537</v>
+        <v>3330771</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Account_8321537</t>
+          <t>Account_3330771</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>8502.15</v>
+        <v>54807.52</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>Admin</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>9086395</v>
+        <v>6200620</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Account_9086395</t>
+          <t>Account_6200620</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>18497.57</v>
+        <v>13517.53</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Accounting</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3898524</v>
+        <v>9294208</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Account_3898524</t>
+          <t>Account_9294208</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>76332.77</v>
+        <v>20051.41</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>Operations</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3594796</v>
+        <v>6662798</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Account_3594796</t>
+          <t>Account_6662798</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17041.65</v>
+        <v>61476.24</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Operations</t>
+          <t>Accounting</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>6226013</v>
+        <v>9861222</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Account_6226013</t>
+          <t>Account_9861222</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>9375.93</v>
+        <v>15815.7</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -972,19 +960,19 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>4322689</v>
+        <v>5823098</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Account_4322689</t>
+          <t>Account_5823098</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>9671.16</v>
+        <v>84016.19</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Admin</t>
         </is>
       </c>
     </row>
@@ -1002,15 +990,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Log_ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Note_ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Operation</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Sync_Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1020,15 +1046,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Override_ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Account_Number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Range_Override</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Effective_Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1038,127 +1102,171 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Map_ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Digit_Position</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Meaning</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Valid_Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Company Code</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SubDept</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cost Center</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Account Type</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Reserved</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Sequence</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0-9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1265,7 +1373,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1285,7 +1393,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>Accounting</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1302,25 +1410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1366,19 +1456,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4322689</v>
+        <v>6200620</v>
       </c>
       <c r="C2" t="n">
-        <v>6302.74</v>
+        <v>6884.16</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Adjustment</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-27</t>
         </is>
       </c>
     </row>
@@ -1387,19 +1477,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>9775371</v>
+        <v>4671827</v>
       </c>
       <c r="C3" t="n">
-        <v>8150.91</v>
+        <v>4909.46</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Adjustment</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-01-22</t>
         </is>
       </c>
     </row>
@@ -1408,19 +1498,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>9086395</v>
+        <v>9294208</v>
       </c>
       <c r="C4" t="n">
-        <v>6934.21</v>
+        <v>5655.32</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Overhead</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -1429,19 +1519,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>8321537</v>
+        <v>4671827</v>
       </c>
       <c r="C5" t="n">
-        <v>3378.38</v>
+        <v>7778.81</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-02-11</t>
         </is>
       </c>
     </row>
@@ -1450,10 +1540,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3038731</v>
+        <v>6662798</v>
       </c>
       <c r="C6" t="n">
-        <v>381.38</v>
+        <v>4616.25</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1462,7 +1552,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-17</t>
         </is>
       </c>
     </row>
@@ -1471,19 +1561,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>8321537</v>
+        <v>7875135</v>
       </c>
       <c r="C7" t="n">
-        <v>1376.94</v>
+        <v>8676.620000000001</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-21</t>
         </is>
       </c>
     </row>
@@ -1492,19 +1582,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>4982845</v>
+        <v>8796304</v>
       </c>
       <c r="C8" t="n">
-        <v>3416.97</v>
+        <v>2352.9</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Overhead</t>
+          <t>Adjustment</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-19</t>
         </is>
       </c>
     </row>
@@ -1513,19 +1603,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>5729196</v>
+        <v>9861222</v>
       </c>
       <c r="C9" t="n">
-        <v>8732.200000000001</v>
+        <v>9281.6</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Adjustment</t>
+          <t>Overhead</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-01-29</t>
         </is>
       </c>
     </row>
@@ -1534,10 +1624,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>9775371</v>
+        <v>2617691</v>
       </c>
       <c r="C10" t="n">
-        <v>5142.07</v>
+        <v>5173.7</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1546,7 +1636,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-26</t>
         </is>
       </c>
     </row>
@@ -1555,19 +1645,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>5100429</v>
+        <v>9294208</v>
       </c>
       <c r="C11" t="n">
-        <v>4467.43</v>
+        <v>6945.47</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Adjustment</t>
+          <t>Overhead</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-07</t>
         </is>
       </c>
     </row>
@@ -1576,19 +1666,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2094202</v>
+        <v>9908228</v>
       </c>
       <c r="C12" t="n">
-        <v>6217.63</v>
+        <v>1049.02</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Adjustment</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
     </row>
@@ -1597,19 +1687,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>4982845</v>
+        <v>4558819</v>
       </c>
       <c r="C13" t="n">
-        <v>3156.74</v>
+        <v>7042.67</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Overhead</t>
+          <t>Adjustment</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-01</t>
         </is>
       </c>
     </row>
@@ -1618,19 +1708,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>9086395</v>
+        <v>7875135</v>
       </c>
       <c r="C14" t="n">
-        <v>3179.77</v>
+        <v>9585.940000000001</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Adjustment</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-02</t>
         </is>
       </c>
     </row>
@@ -1639,19 +1729,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>4551407</v>
+        <v>2617691</v>
       </c>
       <c r="C15" t="n">
-        <v>6679</v>
+        <v>9445.51</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Adjustment</t>
+          <t>Overhead</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-17</t>
         </is>
       </c>
     </row>
@@ -1660,19 +1750,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>9775371</v>
+        <v>6200620</v>
       </c>
       <c r="C16" t="n">
-        <v>7176.54</v>
+        <v>1276.03</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Overhead</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-15</t>
         </is>
       </c>
     </row>
@@ -1681,14 +1771,14 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>8321537</v>
+        <v>9861222</v>
       </c>
       <c r="C17" t="n">
-        <v>6058.86</v>
+        <v>1049.95</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1702,10 +1792,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2981593</v>
+        <v>6662798</v>
       </c>
       <c r="C18" t="n">
-        <v>3949.34</v>
+        <v>5996.2</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1714,7 +1804,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-05</t>
         </is>
       </c>
     </row>
@@ -1723,19 +1813,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>9775371</v>
+        <v>7875135</v>
       </c>
       <c r="C19" t="n">
-        <v>1892.63</v>
+        <v>4488.71</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Adjustment</t>
+          <t>Overhead</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-29</t>
         </is>
       </c>
     </row>
@@ -1744,19 +1834,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1883294</v>
+        <v>2617691</v>
       </c>
       <c r="C20" t="n">
-        <v>3709.07</v>
+        <v>2068.89</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Overhead</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-01-22</t>
         </is>
       </c>
     </row>
@@ -1765,19 +1855,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>4551407</v>
+        <v>4793634</v>
       </c>
       <c r="C21" t="n">
-        <v>2061.75</v>
+        <v>2264.04</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Overhead</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-01-21</t>
         </is>
       </c>
     </row>
@@ -1786,19 +1876,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>5100429</v>
+        <v>4558819</v>
       </c>
       <c r="C22" t="n">
-        <v>748.73</v>
+        <v>275.89</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Overhead</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-01-02</t>
         </is>
       </c>
     </row>
@@ -1807,19 +1897,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>9775371</v>
+        <v>6662798</v>
       </c>
       <c r="C23" t="n">
-        <v>9947.18</v>
+        <v>2647.11</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Adjustment</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-30</t>
         </is>
       </c>
     </row>
@@ -1828,19 +1918,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>2094202</v>
+        <v>7334640</v>
       </c>
       <c r="C24" t="n">
-        <v>1761.94</v>
+        <v>7390.66</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Adjustment</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-06</t>
         </is>
       </c>
     </row>
@@ -1849,10 +1939,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>2981593</v>
+        <v>9908228</v>
       </c>
       <c r="C25" t="n">
-        <v>7486.95</v>
+        <v>730.37</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1861,7 +1951,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-01-27</t>
         </is>
       </c>
     </row>
@@ -1870,19 +1960,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>5293997</v>
+        <v>8066951</v>
       </c>
       <c r="C26" t="n">
-        <v>6795.26</v>
+        <v>2046.82</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Overhead</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-23</t>
         </is>
       </c>
     </row>
@@ -1891,10 +1981,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>8382057</v>
+        <v>6200620</v>
       </c>
       <c r="C27" t="n">
-        <v>779.47</v>
+        <v>4635.78</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1903,7 +1993,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-10</t>
         </is>
       </c>
     </row>
@@ -1912,19 +2002,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>3898524</v>
+        <v>6200620</v>
       </c>
       <c r="C28" t="n">
-        <v>8329.41</v>
+        <v>4280.69</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-02-04</t>
         </is>
       </c>
     </row>
@@ -1933,19 +2023,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>4551407</v>
+        <v>7334640</v>
       </c>
       <c r="C29" t="n">
-        <v>5482.34</v>
+        <v>1030.81</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Overhead</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-15</t>
         </is>
       </c>
     </row>
@@ -1954,10 +2044,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>5293997</v>
+        <v>3330771</v>
       </c>
       <c r="C30" t="n">
-        <v>6222.57</v>
+        <v>5069.26</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1975,19 +2065,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>3898524</v>
+        <v>8066951</v>
       </c>
       <c r="C31" t="n">
-        <v>602.67</v>
+        <v>4532.64</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Adjustment</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-02-06</t>
         </is>
       </c>
     </row>
@@ -1999,7 +2089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2050,11 +2140,11 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4551407</v>
+        <v>6662798</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Comment</t>
+          <t>Internal</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2069,7 +2159,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-01-17</t>
         </is>
       </c>
     </row>
@@ -2078,11 +2168,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>8571538</v>
+        <v>8066951</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Comment</t>
+          <t>Internal</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2092,12 +2182,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>David Brown</t>
+          <t>Bob Smith</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-01-08</t>
         </is>
       </c>
     </row>
@@ -2106,11 +2196,11 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>6226013</v>
+        <v>9294208</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Reconciliation</t>
+          <t>Alert</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2120,12 +2210,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2134,11 +2224,11 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>8382057</v>
+        <v>7023462</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>Reconciliation</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2148,12 +2238,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>David Brown</t>
+          <t>Emma Davis</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-10</t>
         </is>
       </c>
     </row>
@@ -2162,11 +2252,11 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>9086395</v>
+        <v>8066951</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Comment</t>
+          <t>Internal</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2176,12 +2266,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Carol Williams</t>
+          <t>Emma Davis</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-01-21</t>
         </is>
       </c>
     </row>
@@ -2190,11 +2280,11 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>8382057</v>
+        <v>8796304</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Reconciliation</t>
+          <t>Comment</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2204,12 +2294,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Emma Davis</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-09</t>
         </is>
       </c>
     </row>
@@ -2218,11 +2308,11 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2981593</v>
+        <v>4558819</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Comment</t>
+          <t>Reconciliation</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2237,7 +2327,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-04</t>
         </is>
       </c>
     </row>
@@ -2246,11 +2336,11 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>5100429</v>
+        <v>6662798</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>Reconciliation</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2260,12 +2350,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Emma Davis</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-23</t>
         </is>
       </c>
     </row>
@@ -2274,11 +2364,11 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>4982845</v>
+        <v>9861222</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Comment</t>
+          <t>Internal</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2288,12 +2378,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>David Brown</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-01-14</t>
         </is>
       </c>
     </row>
@@ -2302,11 +2392,11 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>5729196</v>
+        <v>4671827</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Reconciliation</t>
+          <t>Alert</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2316,12 +2406,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>David Brown</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-28</t>
         </is>
       </c>
     </row>
@@ -2330,7 +2420,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>5293997</v>
+        <v>7023462</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -2349,7 +2439,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-02</t>
         </is>
       </c>
     </row>
@@ -2358,11 +2448,11 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>8382057</v>
+        <v>5823098</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Alert</t>
+          <t>Comment</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2372,12 +2462,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Carol Williams</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-02-09</t>
         </is>
       </c>
     </row>
@@ -2386,7 +2476,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>8382057</v>
+        <v>6662798</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -2405,7 +2495,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-29</t>
         </is>
       </c>
     </row>
@@ -2414,11 +2504,11 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>8382057</v>
+        <v>4793634</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>Reconciliation</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2428,12 +2518,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Emma Davis</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-02-03</t>
         </is>
       </c>
     </row>
@@ -2442,11 +2532,11 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>4322689</v>
+        <v>9294208</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Alert</t>
+          <t>Reconciliation</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2461,7 +2551,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-02-08</t>
         </is>
       </c>
     </row>
@@ -2470,11 +2560,11 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2981593</v>
+        <v>2511172</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Reconciliation</t>
+          <t>Internal</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2484,12 +2574,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>David Brown</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-02-10</t>
         </is>
       </c>
     </row>
@@ -2498,7 +2588,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>8321537</v>
+        <v>2511172</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -2512,12 +2602,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Emma Davis</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-02-05</t>
         </is>
       </c>
     </row>
@@ -2526,11 +2616,11 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>4551407</v>
+        <v>4558819</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>Comment</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2540,7 +2630,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>David Brown</t>
+          <t>Carol Williams</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2554,11 +2644,11 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>5729196</v>
+        <v>2617691</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Internal</t>
+          <t>Alert</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2568,12 +2658,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-02-03</t>
         </is>
       </c>
     </row>
@@ -2582,11 +2672,11 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>5100429</v>
+        <v>6662798</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Alert</t>
+          <t>Internal</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2596,12 +2686,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Carol Williams</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-02-03</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2712,7 +2802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2819,7 +2909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2927,7 +3017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2978,7 +3068,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3594796</v>
+        <v>8796304</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2987,12 +3077,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -3006,7 +3096,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3038731</v>
+        <v>2617691</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -3015,12 +3105,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -3034,7 +3124,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>5729196</v>
+        <v>3330771</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -3043,12 +3133,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Low</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3062,7 +3152,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>8382057</v>
+        <v>6662798</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -3076,7 +3166,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3090,7 +3180,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5729196</v>
+        <v>5823098</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -3104,7 +3194,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -3121,13 +3211,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3162,404 +3252,17 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Log_ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Note_ID</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Operation</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Result</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Sync_Date</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Override_ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Account_Number</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Range_Override</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Reason</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Effective_Date</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Map_ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Digit_Position</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Meaning</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Valid_Values</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Company Code</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1-9</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Department</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0-9</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>SubDept</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0-9</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Cost Center</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0-9</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Account Type</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0-9</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Reserved</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0-9</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Sequence</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0-9</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>